<commit_message>
...up to selection of grains
</commit_message>
<xml_diff>
--- a/Database/Brewing_Constants.xlsx
+++ b/Database/Brewing_Constants.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7350" tabRatio="683" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7350" tabRatio="683" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Grains" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Yeast" sheetId="3" r:id="rId5"/>
     <sheet name="Styles" sheetId="4" r:id="rId6"/>
     <sheet name="Spices" sheetId="7" r:id="rId7"/>
+    <sheet name="SystemSpecificInformation" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2732" uniqueCount="1816">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2740" uniqueCount="1824">
   <si>
     <t>Ingredients</t>
   </si>
@@ -5992,6 +5993,30 @@
   </si>
   <si>
     <t>AlcoholTolerancePercent</t>
+  </si>
+  <si>
+    <t>BatchSize[Gal]</t>
+  </si>
+  <si>
+    <t>EvapRate[Percent_per_hr]</t>
+  </si>
+  <si>
+    <t>ShrinkageFromCooling[Percent]</t>
+  </si>
+  <si>
+    <t>BrewHouseEfficiency[Percent]</t>
+  </si>
+  <si>
+    <t>WeightOfMashTun[lb]</t>
+  </si>
+  <si>
+    <t>ThermalMassOfMAshTun[btu_per_(lb*DegreeF)]</t>
+  </si>
+  <si>
+    <t>BoilKettleDeadSpace[Gal]</t>
+  </si>
+  <si>
+    <t>LauterTunDeadSpace[Gal]</t>
   </si>
 </sst>
 </file>
@@ -14248,7 +14273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -21655,4 +21680,81 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1817</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1818</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1819</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1820</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1821</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1822</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>5.5</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>70</v>
+      </c>
+      <c r="E2">
+        <v>7.5</v>
+      </c>
+      <c r="F2">
+        <v>0.38</v>
+      </c>
+      <c r="G2">
+        <v>0.5</v>
+      </c>
+      <c r="H2">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Database Update... -Added Gravity Correction Chart -Modified Spices to have fewer cols -Changed Database load file
</commit_message>
<xml_diff>
--- a/Database/Brewing_Constants.xlsx
+++ b/Database/Brewing_Constants.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7350" tabRatio="683" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7350" tabRatio="785" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Grains" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Styles" sheetId="4" r:id="rId6"/>
     <sheet name="Spices" sheetId="7" r:id="rId7"/>
     <sheet name="SystemSpecificInformation" sheetId="8" r:id="rId8"/>
+    <sheet name="Gravity_Correction_Chart" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2748" uniqueCount="1828">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2746" uniqueCount="1831">
   <si>
     <t>Ingredients</t>
   </si>
@@ -6032,6 +6033,15 @@
   </si>
   <si>
     <t>Treacle is any syrup made during the refining of sugar and is defined as \ uncrystallized syrup produced in refining sugar\.</t>
+  </si>
+  <si>
+    <t>Temperature_F</t>
+  </si>
+  <si>
+    <t>Temperature_C</t>
+  </si>
+  <si>
+    <t>Add_SG</t>
   </si>
 </sst>
 </file>
@@ -22085,26 +22095,20 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" activeCellId="1" sqref="A1 A19:XFD19"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="12.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="2" width="12.7265625" style="1"/>
+    <col min="3" max="3" width="255.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="12.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>1673</v>
       </c>
@@ -22112,73 +22116,43 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>1787</v>
-      </c>
-      <c r="D1" s="7" t="s">
         <v>1786</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>1788</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>1789</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>1621</v>
       </c>
       <c r="B2" s="8">
         <v>114</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="8" t="s">
         <v>1622</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>1623</v>
       </c>
       <c r="B3" s="8">
         <v>115</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="8" t="s">
         <v>1624</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>1625</v>
       </c>
       <c r="B4" s="8">
         <v>116</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8" t="s">
+      <c r="C4" s="8" t="s">
         <v>1626</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>1627</v>
       </c>
@@ -22186,93 +22160,63 @@
         <v>117</v>
       </c>
       <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="6"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>1628</v>
       </c>
       <c r="B6" s="8">
         <v>118</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8" t="s">
+      <c r="C6" s="8" t="s">
         <v>1629</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>1630</v>
       </c>
       <c r="B7" s="8">
         <v>119</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="8" t="s">
         <v>1631</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>1632</v>
       </c>
       <c r="B8" s="8">
         <v>120</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="8" t="s">
         <v>1633</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>1634</v>
       </c>
       <c r="B9" s="8">
         <v>121</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8" t="s">
+      <c r="C9" s="8" t="s">
         <v>1635</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>1636</v>
       </c>
       <c r="B10" s="8">
         <v>122</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8" t="s">
+      <c r="C10" s="8" t="s">
         <v>1637</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>1638</v>
       </c>
@@ -22280,61 +22224,41 @@
         <v>123</v>
       </c>
       <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>1639</v>
       </c>
       <c r="B12" s="8">
         <v>124</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8" t="s">
+      <c r="C12" s="8" t="s">
         <v>1640</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>1641</v>
       </c>
       <c r="B13" s="8">
         <v>125</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8" t="s">
+      <c r="C13" s="8" t="s">
         <v>1642</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="6"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>1643</v>
       </c>
       <c r="B14" s="8">
         <v>126</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8" t="s">
+      <c r="C14" s="8" t="s">
         <v>1644</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
         <v>1645</v>
       </c>
@@ -22342,45 +22266,30 @@
         <v>127</v>
       </c>
       <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>1646</v>
       </c>
       <c r="B16" s="8">
         <v>128</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8" t="s">
+      <c r="C16" s="8" t="s">
         <v>1647</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="6"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>1648</v>
       </c>
       <c r="B17" s="8">
         <v>129</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8" t="s">
+      <c r="C17" s="8" t="s">
         <v>1649</v>
       </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="6"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
         <v>1650</v>
       </c>
@@ -22388,13 +22297,8 @@
         <v>130</v>
       </c>
       <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="6"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>1651</v>
       </c>
@@ -22402,13 +22306,8 @@
         <v>131</v>
       </c>
       <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="6"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
         <v>1652</v>
       </c>
@@ -22416,13 +22315,8 @@
         <v>132</v>
       </c>
       <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="6"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
         <v>1653</v>
       </c>
@@ -22430,13 +22324,8 @@
         <v>133</v>
       </c>
       <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="6"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
         <v>1654</v>
       </c>
@@ -22444,45 +22333,30 @@
         <v>134</v>
       </c>
       <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="6"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
         <v>1655</v>
       </c>
       <c r="B23" s="8">
         <v>135</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8" t="s">
+      <c r="C23" s="8" t="s">
         <v>1656</v>
       </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="6"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
         <v>1657</v>
       </c>
       <c r="B24" s="8">
         <v>136</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8" t="s">
+      <c r="C24" s="8" t="s">
         <v>1658</v>
       </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="6"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
         <v>1659</v>
       </c>
@@ -22490,13 +22364,8 @@
         <v>137</v>
       </c>
       <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="6"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
         <v>1660</v>
       </c>
@@ -22504,13 +22373,8 @@
         <v>138</v>
       </c>
       <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="6"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
         <v>1661</v>
       </c>
@@ -22518,13 +22382,8 @@
         <v>139</v>
       </c>
       <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="6"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
         <v>1662</v>
       </c>
@@ -22532,13 +22391,8 @@
         <v>140</v>
       </c>
       <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="6"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="8" t="s">
         <v>1663</v>
       </c>
@@ -22546,13 +22400,8 @@
         <v>141</v>
       </c>
       <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="6"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
         <v>1664</v>
       </c>
@@ -22560,13 +22409,8 @@
         <v>142</v>
       </c>
       <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="6"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="8" t="s">
         <v>1665</v>
       </c>
@@ -22574,13 +22418,8 @@
         <v>143</v>
       </c>
       <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="6"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="8" t="s">
         <v>1666</v>
       </c>
@@ -22588,13 +22427,8 @@
         <v>144</v>
       </c>
       <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="6"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="8" t="s">
         <v>1667</v>
       </c>
@@ -22602,13 +22436,8 @@
         <v>145</v>
       </c>
       <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="6"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="8" t="s">
         <v>1668</v>
       </c>
@@ -22616,13 +22445,8 @@
         <v>146</v>
       </c>
       <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="6"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="8" t="s">
         <v>1669</v>
       </c>
@@ -22630,13 +22454,8 @@
         <v>147</v>
       </c>
       <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="6"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="8" t="s">
         <v>1670</v>
       </c>
@@ -22644,13 +22463,8 @@
         <v>148</v>
       </c>
       <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="6"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="8" t="s">
         <v>1671</v>
       </c>
@@ -22658,13 +22472,8 @@
         <v>149</v>
       </c>
       <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="6"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="8" t="s">
         <v>1672</v>
       </c>
@@ -22672,11 +22481,6 @@
         <v>150</v>
       </c>
       <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22758,4 +22562,167 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1828</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1829</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>80</v>
+      </c>
+      <c r="B2">
+        <v>27</v>
+      </c>
+      <c r="C2">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>90</v>
+      </c>
+      <c r="B3">
+        <v>32</v>
+      </c>
+      <c r="C3">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4">
+        <v>38</v>
+      </c>
+      <c r="C4">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>110</v>
+      </c>
+      <c r="B5">
+        <v>43</v>
+      </c>
+      <c r="C5">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>120</v>
+      </c>
+      <c r="B6">
+        <v>49</v>
+      </c>
+      <c r="C6">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>130</v>
+      </c>
+      <c r="B7">
+        <v>54</v>
+      </c>
+      <c r="C7">
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>140</v>
+      </c>
+      <c r="B8">
+        <v>60</v>
+      </c>
+      <c r="C8">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>150</v>
+      </c>
+      <c r="B9">
+        <v>66</v>
+      </c>
+      <c r="C9">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>160</v>
+      </c>
+      <c r="B10">
+        <v>71</v>
+      </c>
+      <c r="C10">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>170</v>
+      </c>
+      <c r="B11">
+        <v>77</v>
+      </c>
+      <c r="C11">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>190</v>
+      </c>
+      <c r="B12">
+        <v>88</v>
+      </c>
+      <c r="C12">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>212</v>
+      </c>
+      <c r="B13">
+        <v>100</v>
+      </c>
+      <c r="C13">
+        <v>0.04</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>